<commit_message>
Added notebook on Hashing with images
</commit_message>
<xml_diff>
--- a/Data-structures.xlsx
+++ b/Data-structures.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="113">
   <si>
     <t>Array Data structure</t>
   </si>
@@ -339,6 +339,21 @@
   </si>
   <si>
     <t>After 4th Iteration</t>
+  </si>
+  <si>
+    <t>Hashing:</t>
+  </si>
+  <si>
+    <t>Using a Data Structure that employs a hash function allows you to do look-ups in constant time.</t>
+  </si>
+  <si>
+    <t>In lists or set, you need to look through every element to find the one you are looking for. This makes the look up in linear time instead of constant time.</t>
+  </si>
+  <si>
+    <t>Stacks and Queues lets you look-up oldest or newest element immediately, while Priority queues will let you find the highest priority element quickly. For any other elements, you need to do linear time search.</t>
+  </si>
+  <si>
+    <t>Constant time look-ups makes the algorithms faster.</t>
   </si>
 </sst>
 </file>
@@ -346,10 +361,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -368,22 +383,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -398,29 +400,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -428,47 +415,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -490,8 +437,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -504,9 +490,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -581,181 +596,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,6 +781,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -817,21 +847,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -852,16 +867,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -871,148 +886,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="41" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2369,10 +2384,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X73"/>
+  <dimension ref="A1:X80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2"/>
@@ -2431,7 +2446,6 @@
       <c r="A8" t="s">
         <v>49</v>
       </c>
-      <c r="B8"/>
       <c r="C8">
         <v>3</v>
       </c>
@@ -2809,7 +2823,6 @@
       <c r="B48" t="s">
         <v>73</v>
       </c>
-      <c r="C48"/>
       <c r="D48" t="s">
         <v>74</v>
       </c>
@@ -3212,6 +3225,31 @@
       </c>
       <c r="H73">
         <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added content of BST and Heaps
</commit_message>
<xml_diff>
--- a/Data-structures.xlsx
+++ b/Data-structures.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="204">
   <si>
     <t>Array Data structure</t>
   </si>
@@ -368,12 +368,27 @@
     <t>Leaf</t>
   </si>
   <si>
+    <t>Search and Delete</t>
+  </si>
+  <si>
+    <t>Since, we may need to traverse all elements for search. And delete also requires search.</t>
+  </si>
+  <si>
     <t>Internal</t>
   </si>
   <si>
     <t>External</t>
   </si>
   <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>(logn)</t>
+  </si>
+  <si>
+    <t>Since the nodes increase in exponents of 2 at every level.</t>
+  </si>
+  <si>
     <t>Parent</t>
   </si>
   <si>
@@ -405,6 +420,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Pre-Order</t>
     </r>
     <r>
@@ -426,6 +449,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>In-Order</t>
     </r>
     <r>
@@ -444,6 +475,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Post-Order</t>
     </r>
     <r>
@@ -503,15 +542,15 @@
     <t>While deleting a node, one of the leaf node can take place of the deleted node, since no fixed order of elements is required.</t>
   </si>
   <si>
-    <t>Insert</t>
-  </si>
-  <si>
     <t>Just follow the two children rule. Find an open spot and insert the new node there. Insertion can be in some internal node which has only 1 children, or at some leaf node.</t>
   </si>
   <si>
     <t>Insertion time complexity depends on height of the tree.</t>
   </si>
   <si>
+    <t>O(logn)</t>
+  </si>
+  <si>
     <t>Perfect Tree</t>
   </si>
   <si>
@@ -537,6 +576,117 @@
   </si>
   <si>
     <t>Every value on the left of the node is smaller than it. Every value on the right of the node is larger than it.</t>
+  </si>
+  <si>
+    <t>Search process depends on height of tree.</t>
+  </si>
+  <si>
+    <t>Deleting faces same complications as generic trees</t>
+  </si>
+  <si>
+    <t>Unbalanced BST</t>
+  </si>
+  <si>
+    <t>Not all parents have two children each.</t>
+  </si>
+  <si>
+    <t>Worst</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Consider an example where every parent has just one child, which is greater than it, so placed on right. This goes on to the depth of tree.</t>
+  </si>
+  <si>
+    <t>Called unbalanced as the distribution is skewed towards right or left.</t>
+  </si>
+  <si>
+    <t>Skewing could take place at one of the sub-trees as well.</t>
+  </si>
+  <si>
+    <t>Search, Insert and Delete takes linear time for Unbalanced BST, so it can be considered as worst case scenario of BST.</t>
+  </si>
+  <si>
+    <t>Heap (Tree)</t>
+  </si>
+  <si>
+    <t>Elements are arranged in increasing or decreasing order such that the root element is either the maximum or the minimum value in the tree.</t>
+  </si>
+  <si>
+    <t>Max heaps have parents as greater value than their child while Min heaps are vice-versa.</t>
+  </si>
+  <si>
+    <t>Heaps do not need to be Binary Tree so a parent can have any number of children.</t>
+  </si>
+  <si>
+    <t>Search, Insert and Delete vary a lot based on the type of heap.</t>
+  </si>
+  <si>
+    <t>Max Binary Heap</t>
+  </si>
+  <si>
+    <t>Max Heap following rules of Binary Tree</t>
+  </si>
+  <si>
+    <t>Complete Tree: so other than leaves, all other nodes must have 2 children.</t>
+  </si>
+  <si>
+    <t>The values are added from left to right, till the level is not full.</t>
+  </si>
+  <si>
+    <t>Peek function gets maximum value and it happens in constant time O(1)</t>
+  </si>
+  <si>
+    <t>Search becomes linear time</t>
+  </si>
+  <si>
+    <t>Trick</t>
+  </si>
+  <si>
+    <t>Don't check anything in sub-tree if the search value is bigger than a node value</t>
+  </si>
+  <si>
+    <t>Search Worst Case</t>
+  </si>
+  <si>
+    <t>Search Average Case</t>
+  </si>
+  <si>
+    <t>O(n\2)</t>
+  </si>
+  <si>
+    <t>Stick the new element in the next open slot of the tree and then Heapify.</t>
+  </si>
+  <si>
+    <t>Heapify</t>
+  </si>
+  <si>
+    <t>Heapify is the operation in which we reoder the tree based on the heap property.</t>
+  </si>
+  <si>
+    <t>Compare the new element with parent and swap them when the child is bigger.</t>
+  </si>
+  <si>
+    <t>Extract</t>
+  </si>
+  <si>
+    <t>In extract operation, we remove the root from the tree.</t>
+  </si>
+  <si>
+    <t>Here also, we stick the rightmost leaf in the root spot and then just compare it to its children and swap where necessary.</t>
+  </si>
+  <si>
+    <t>Insert, Delete, general case of Extract</t>
+  </si>
+  <si>
+    <t>Worst Case</t>
+  </si>
+  <si>
+    <t>Considering height of tree.</t>
+  </si>
+  <si>
+    <t>The worst case would be moving an element all the way up or down the tree and would roughly be as many operations as the height of the tree.</t>
   </si>
 </sst>
 </file>
@@ -544,10 +694,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -566,61 +716,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -635,7 +733,90 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -650,10 +831,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -664,47 +845,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -779,7 +929,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -791,7 +941,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,49 +1031,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,37 +1067,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,25 +1079,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,25 +1091,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,12 +1132,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1004,45 +1167,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1075,7 +1199,33 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1084,152 +1234,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1261,6 +1411,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1785,13 +1938,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -1801,7 +1954,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3360420" y="20678775"/>
+          <a:off x="3360420" y="20836890"/>
           <a:ext cx="662940" cy="184785"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1832,13 +1985,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -1848,7 +2001,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4709160" y="20686395"/>
+          <a:off x="4709160" y="20844510"/>
           <a:ext cx="662940" cy="184785"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1879,13 +2032,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -1895,7 +2048,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2697480" y="21065490"/>
+          <a:off x="2697480" y="21223605"/>
           <a:ext cx="312420" cy="160020"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1926,13 +2079,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -1942,7 +2095,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2994660" y="21040725"/>
+          <a:off x="2994660" y="21198840"/>
           <a:ext cx="358140" cy="161925"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1973,13 +2126,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>124</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -1989,7 +2142,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5394960" y="21040725"/>
+          <a:off x="5394960" y="21198840"/>
           <a:ext cx="327660" cy="169545"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2020,13 +2173,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>5715</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>5715</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -2036,8 +2189,149 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5737860" y="21055965"/>
+          <a:off x="5737860" y="21214080"/>
           <a:ext cx="297180" cy="177165"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038600" y="23086695"/>
+          <a:ext cx="632460" cy="154305"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5387340" y="23418165"/>
+          <a:ext cx="640080" cy="177165"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6522720" y="23764875"/>
+          <a:ext cx="632460" cy="192405"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2333,10 +2627,10 @@
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="10.2" customWidth="1"/>
-    <col min="2" max="2" width="18" style="12" customWidth="1"/>
-    <col min="3" max="3" width="8.8" style="12"/>
-    <col min="4" max="4" width="10.3" style="12" customWidth="1"/>
-    <col min="5" max="8" width="8.8" style="12"/>
+    <col min="2" max="2" width="18" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.8" style="10"/>
+    <col min="4" max="4" width="10.3" style="10" customWidth="1"/>
+    <col min="5" max="8" width="8.8" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2348,7 +2642,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2356,25 +2650,25 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2382,22 +2676,22 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2405,25 +2699,25 @@
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>0</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>2</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="16">
         <v>3</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="16">
         <v>4</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="16">
         <v>5</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="10">
         <v>6</v>
       </c>
     </row>
@@ -2436,7 +2730,7 @@
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2444,25 +2738,25 @@
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2470,25 +2764,25 @@
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2496,25 +2790,25 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>0</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <v>1</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <v>2</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="17">
         <v>3</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="16">
         <v>4</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="16">
         <v>5</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="16">
         <v>6</v>
       </c>
     </row>
@@ -2527,7 +2821,7 @@
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2535,22 +2829,22 @@
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2558,22 +2852,22 @@
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2581,22 +2875,22 @@
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2609,25 +2903,25 @@
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2635,25 +2929,25 @@
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2661,25 +2955,25 @@
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2692,7 +2986,7 @@
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2700,22 +2994,22 @@
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2723,22 +3017,22 @@
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2746,22 +3040,22 @@
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2777,7 +3071,7 @@
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="15" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2785,25 +3079,25 @@
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G34" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="H34" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2811,25 +3105,25 @@
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F35" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="H35" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2837,25 +3131,25 @@
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="H36" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2863,10 +3157,10 @@
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2874,7 +3168,7 @@
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2882,22 +3176,22 @@
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="G40" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2905,22 +3199,22 @@
       <c r="A41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="G41" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2928,22 +3222,22 @@
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="12" t="s">
+      <c r="G42" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2956,13 +3250,13 @@
       <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G45" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2970,25 +3264,25 @@
       <c r="A46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G46" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H46" s="12" t="s">
+      <c r="H46" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2996,25 +3290,25 @@
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G47" s="12" t="s">
+      <c r="G47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="12" t="s">
+      <c r="H47" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3022,25 +3316,25 @@
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G48" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H48" s="12" t="s">
+      <c r="H48" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3053,13 +3347,13 @@
       <c r="A51" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D51" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G51" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3067,25 +3361,25 @@
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G52" s="12" t="s">
+      <c r="G52" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H52" s="12" t="s">
+      <c r="H52" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K52" t="s">
@@ -3096,25 +3390,25 @@
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G53" s="12" t="s">
+      <c r="G53" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H53" s="12" t="s">
+      <c r="H53" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3122,25 +3416,25 @@
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="18" t="s">
+      <c r="C54" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G54" s="12" t="s">
+      <c r="G54" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H54" s="12" t="s">
+      <c r="H54" s="10" t="s">
         <v>26</v>
       </c>
       <c r="K54" t="s">
@@ -3157,10 +3451,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X127"/>
+  <dimension ref="A1:X167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2"/>
@@ -4025,7 +4319,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>113</v>
       </c>
@@ -4038,82 +4332,101 @@
       <c r="D82" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="83" spans="2:4">
+      <c r="F82" t="s">
+        <v>117</v>
+      </c>
+      <c r="G82"/>
+      <c r="H82" t="s">
+        <v>86</v>
+      </c>
+      <c r="I82" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9">
       <c r="B83" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C83" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D83" t="s">
-        <v>118</v>
+        <v>120</v>
+      </c>
+      <c r="F83" t="s">
+        <v>121</v>
+      </c>
+      <c r="H83" t="s">
+        <v>122</v>
+      </c>
+      <c r="I83" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="B84" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C84" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D84" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="B85" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C85" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D85" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B87" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D87" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="B88" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="4:4">
       <c r="D89" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="4:4">
       <c r="D90" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="4:4">
       <c r="D91" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="4:4">
       <c r="D92" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="4:4">
       <c r="D93" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="95" ht="13.95" spans="4:9">
@@ -4150,7 +4463,7 @@
       <c r="E98" s="10"/>
       <c r="G98" s="10"/>
       <c r="H98" s="11" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="I98" s="10"/>
     </row>
@@ -4171,51 +4484,51 @@
         <v>14</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="11" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103" spans="3:4">
       <c r="C103" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D103" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="3:4">
       <c r="C104" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D104" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="105" spans="3:4">
       <c r="C105" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D105" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B107" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="108" spans="2:11">
       <c r="B108" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D108" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="K108" t="s">
         <v>86</v>
@@ -4223,10 +4536,10 @@
     </row>
     <row r="109" spans="2:15">
       <c r="B109" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D109" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="O109" t="s">
         <v>86</v>
@@ -4234,109 +4547,367 @@
     </row>
     <row r="110" spans="2:4">
       <c r="B110" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D110" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="111" spans="4:4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="111" spans="4:10">
       <c r="D111" t="s">
-        <v>152</v>
+        <v>156</v>
+      </c>
+      <c r="J111" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="113" spans="2:4">
       <c r="B113" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D113" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="114" spans="4:4">
       <c r="D114" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B116" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C118" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="122" ht="13.95"/>
-    <row r="123" ht="13.95" spans="4:9">
-      <c r="D123" s="10"/>
-      <c r="E123" s="10"/>
-      <c r="F123" s="11">
-        <v>4</v>
-      </c>
-      <c r="G123" s="10"/>
-      <c r="H123" s="10"/>
-      <c r="I123" s="10"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="121" spans="3:7">
+      <c r="C121" t="s">
+        <v>167</v>
+      </c>
+      <c r="G121" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3">
+      <c r="C122" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="124" ht="13.95" spans="4:9">
       <c r="D124" s="10"/>
       <c r="E124" s="10"/>
-      <c r="F124" s="10"/>
+      <c r="F124" s="11">
+        <v>4</v>
+      </c>
       <c r="G124" s="10"/>
       <c r="H124" s="10"/>
       <c r="I124" s="10"/>
     </row>
-    <row r="125" ht="13.95" spans="3:9">
-      <c r="C125" s="10"/>
-      <c r="D125" s="11">
-        <v>2</v>
-      </c>
+    <row r="125" ht="13.95" spans="4:9">
+      <c r="D125" s="10"/>
       <c r="E125" s="10"/>
+      <c r="F125" s="10"/>
       <c r="G125" s="10"/>
-      <c r="H125" s="11">
-        <v>6</v>
-      </c>
+      <c r="H125" s="10"/>
       <c r="I125" s="10"/>
     </row>
     <row r="126" ht="13.95" spans="3:9">
       <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
+      <c r="D126" s="11">
+        <v>2</v>
+      </c>
       <c r="E126" s="10"/>
       <c r="G126" s="10"/>
-      <c r="H126" s="10"/>
+      <c r="H126" s="11">
+        <v>6</v>
+      </c>
       <c r="I126" s="10"/>
     </row>
     <row r="127" ht="13.95" spans="3:9">
-      <c r="C127" s="11">
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+      <c r="G127" s="10"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+    </row>
+    <row r="128" ht="13.95" spans="3:9">
+      <c r="C128" s="11">
         <v>1</v>
       </c>
-      <c r="D127" s="10"/>
-      <c r="E127" s="11">
+      <c r="D128" s="10"/>
+      <c r="E128" s="11">
         <v>3</v>
       </c>
-      <c r="G127" s="11">
+      <c r="G128" s="11">
         <v>5</v>
       </c>
-      <c r="H127" s="10"/>
-      <c r="I127" s="11">
+      <c r="H128" s="10"/>
+      <c r="I128" s="11">
         <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" t="s">
+        <v>169</v>
+      </c>
+      <c r="C131" t="s">
+        <v>170</v>
+      </c>
+      <c r="G131" t="s">
+        <v>171</v>
+      </c>
+      <c r="H131" t="s">
+        <v>86</v>
+      </c>
+      <c r="J131" t="s">
+        <v>172</v>
+      </c>
+      <c r="K131" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3">
+      <c r="C132" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3">
+      <c r="C133" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3">
+      <c r="C134" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3">
+      <c r="C135" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="137" ht="13.95" spans="5:11">
+      <c r="E137" s="12">
+        <v>5</v>
+      </c>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="13"/>
+      <c r="J137" s="13"/>
+      <c r="K137" s="13"/>
+    </row>
+    <row r="138" ht="13.95" spans="5:11">
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="13"/>
+      <c r="I138" s="13"/>
+      <c r="J138" s="13"/>
+      <c r="K138" s="13"/>
+    </row>
+    <row r="139" ht="13.95" spans="5:11">
+      <c r="E139" s="13"/>
+      <c r="F139" s="13"/>
+      <c r="G139" s="12">
+        <v>7</v>
+      </c>
+      <c r="H139" s="13"/>
+      <c r="I139" s="13"/>
+      <c r="J139" s="13"/>
+      <c r="K139" s="13"/>
+    </row>
+    <row r="140" ht="13.95" spans="5:11">
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="13"/>
+      <c r="J140" s="13"/>
+      <c r="K140" s="13"/>
+    </row>
+    <row r="141" ht="13.95" spans="5:11">
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="12">
+        <v>9</v>
+      </c>
+      <c r="J141" s="13"/>
+      <c r="K141" s="13"/>
+    </row>
+    <row r="142" ht="13.95" spans="5:11">
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+      <c r="I142" s="13"/>
+      <c r="J142" s="13"/>
+      <c r="K142" s="13"/>
+    </row>
+    <row r="143" ht="13.95" spans="5:11">
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+      <c r="I143" s="13"/>
+      <c r="J143" s="13"/>
+      <c r="K143" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>177</v>
+      </c>
+      <c r="B146" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>182</v>
+      </c>
+      <c r="B151" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2">
+      <c r="B152" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5">
+      <c r="B155" t="s">
+        <v>187</v>
+      </c>
+      <c r="E155" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3">
+      <c r="B156" t="s">
+        <v>188</v>
+      </c>
+      <c r="C156" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5">
+      <c r="B157" t="s">
+        <v>190</v>
+      </c>
+      <c r="C157"/>
+      <c r="E157" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5">
+      <c r="B158" t="s">
+        <v>191</v>
+      </c>
+      <c r="E158" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3">
+      <c r="B160" t="s">
+        <v>121</v>
+      </c>
+      <c r="C160" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3">
+      <c r="B161" t="s">
+        <v>194</v>
+      </c>
+      <c r="C161" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3">
+      <c r="C162" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3">
+      <c r="B163" t="s">
+        <v>197</v>
+      </c>
+      <c r="C163" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3">
+      <c r="C164" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="166" spans="2:10">
+      <c r="B166" t="s">
+        <v>200</v>
+      </c>
+      <c r="F166" t="s">
+        <v>201</v>
+      </c>
+      <c r="H166" t="s">
+        <v>157</v>
+      </c>
+      <c r="J166" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added content of Self-Balancing Trees
</commit_message>
<xml_diff>
--- a/Data-structures.xlsx
+++ b/Data-structures.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="254">
   <si>
     <t>Array Data structure</t>
   </si>
@@ -608,6 +608,9 @@
     <t>Search, Insert and Delete takes linear time for Unbalanced BST, so it can be considered as worst case scenario of BST.</t>
   </si>
   <si>
+    <t>The extreme case of unbalanced tree can be thought of as a linked list. This is depicted below.</t>
+  </si>
+  <si>
     <t>Heap (Tree)</t>
   </si>
   <si>
@@ -687,6 +690,153 @@
   </si>
   <si>
     <t>The worst case would be moving an element all the way up or down the tree and would roughly be as many operations as the height of the tree.</t>
+  </si>
+  <si>
+    <t>Heap Implementations</t>
+  </si>
+  <si>
+    <t>Though heaps are represented as Trees, they are often stored as arrays.</t>
+  </si>
+  <si>
+    <t>Since we know that each node has 2 children and how many nodes will be at each level, this information helps as store the tree into array.</t>
+  </si>
+  <si>
+    <t>Main idea here is that the data should be sorted in descending or ascending order for max or min heap respectively.</t>
+  </si>
+  <si>
+    <t>Tree Level</t>
+  </si>
+  <si>
+    <t>Tree Node</t>
+  </si>
+  <si>
+    <t>Storing the heap as array saves space as we don't need to store pointers to child and parents</t>
+  </si>
+  <si>
+    <t>And data insertion, retrieval can be done easily by computing index based on heap logic.</t>
+  </si>
+  <si>
+    <t>Left Child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Child </t>
+  </si>
+  <si>
+    <t>Self-Balancing Trees:</t>
+  </si>
+  <si>
+    <t>A self-balancing tree tries to minimize the number of levels that it uses.</t>
+  </si>
+  <si>
+    <t>It does some kind algorithm during the insertion and deletion to keep itself balanced and the nodes themselves might have some additional properties.</t>
+  </si>
+  <si>
+    <t>The most common example is a red-black tree, which is an extension of binary search tree.</t>
+  </si>
+  <si>
+    <t>Red-Black Tree</t>
+  </si>
+  <si>
+    <t>The nodes are assigned additional color property, either red or black.</t>
+  </si>
+  <si>
+    <t>There also exists null leaf nodes. All null leaf nodes must be colored black.</t>
+  </si>
+  <si>
+    <t>If a node is red, both of its children must be black.</t>
+  </si>
+  <si>
+    <t>The root node must be black. (Optional Rule)</t>
+  </si>
+  <si>
+    <t>Every path from a node to its descendant null nodes must contain the same number of black nodes. This rules contribute to balancing.</t>
+  </si>
+  <si>
+    <t>Insertion:</t>
+  </si>
+  <si>
+    <t>You should try to insert a node as a red node</t>
+  </si>
+  <si>
+    <t>Case 1:</t>
+  </si>
+  <si>
+    <t>Inserting the first node, i.e. Root.</t>
+  </si>
+  <si>
+    <t>Insert it as Red. It can be changed to black considering optional rule 4.</t>
+  </si>
+  <si>
+    <t>Case 2:</t>
+  </si>
+  <si>
+    <t>Inserting a node at 2nd level.</t>
+  </si>
+  <si>
+    <t>Since it's parent is already black (root is black), no change is needed there.</t>
+  </si>
+  <si>
+    <t>This node will remain red and it won't upset the balance of the tree.</t>
+  </si>
+  <si>
+    <t>Case 3:</t>
+  </si>
+  <si>
+    <t>You insert a node at 3rd level whose parent is red at 2nd level.</t>
+  </si>
+  <si>
+    <t>Rule: If a parent and it's sibling, both are red, then they should be turned to black and the grandparent becomes red.</t>
+  </si>
+  <si>
+    <t>Node colors are switched in this way to maintain the number of black nodes in a given path.</t>
+  </si>
+  <si>
+    <t>The grandparent color can be changed back to black considering rule 4. Still the total number of black nodes on each path will remain same.</t>
+  </si>
+  <si>
+    <t>Case 4:</t>
+  </si>
+  <si>
+    <t>Node parent is red and it's sibling is black. You need to perform a rotation in such case.</t>
+  </si>
+  <si>
+    <t>In a rotation, you shift a group of nodes around in a way that changes the structure of the tree, but not the order of the nodes.</t>
+  </si>
+  <si>
+    <t>Left Rotation</t>
+  </si>
+  <si>
+    <t>Node shifts one place to the left</t>
+  </si>
+  <si>
+    <t>A left rotation would lead to case 5</t>
+  </si>
+  <si>
+    <t>Case 5:</t>
+  </si>
+  <si>
+    <t>Red node and red parent are on the same side of their parents.</t>
+  </si>
+  <si>
+    <t>Now we do the righ rotation, involving the grand parent as well.</t>
+  </si>
+  <si>
+    <t>This will make sure the exact number of black nodes on every path.</t>
+  </si>
+  <si>
+    <t>In doing the rotations, we kept any one sub-tree from getting much larger than the other.</t>
+  </si>
+  <si>
+    <t>Insert, Search and Delete</t>
+  </si>
+  <si>
+    <t>Average and Worst Case</t>
+  </si>
+  <si>
+    <t>BST were O(n) in worst cases because they could be unbalanced.</t>
+  </si>
+  <si>
+    <t>Because of the balance, the run time does not grow so much.</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1127,6 +1277,137 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1264,7 +1545,7 @@
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1306,10 +1587,10 @@
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1318,28 +1599,28 @@
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1360,13 +1641,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1379,7 +1660,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1416,10 +1697,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2220,13 +2531,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>5715</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>632460</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -2236,7 +2547,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4038600" y="23086695"/>
+          <a:off x="4038600" y="23254335"/>
           <a:ext cx="632460" cy="154305"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2267,13 +2578,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>139</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -2283,7 +2594,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5387340" y="23418165"/>
+          <a:off x="5387340" y="23585805"/>
           <a:ext cx="640080" cy="177165"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2314,13 +2625,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>624840</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
@@ -2330,8 +2641,384 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6522720" y="23764875"/>
+          <a:off x="6522720" y="23932515"/>
           <a:ext cx="632460" cy="192405"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4046220" y="30179010"/>
+          <a:ext cx="1303020" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2727960" y="30533340"/>
+          <a:ext cx="609600" cy="177165"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2049780" y="30912435"/>
+          <a:ext cx="312420" cy="160020"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2354580" y="30912435"/>
+          <a:ext cx="304800" cy="144780"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038600" y="30540960"/>
+          <a:ext cx="647700" cy="154305"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6065520" y="30163770"/>
+          <a:ext cx="1112520" cy="207645"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6537960" y="30533340"/>
+          <a:ext cx="655320" cy="169545"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp>
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7879080" y="30548580"/>
+          <a:ext cx="640080" cy="146685"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2642,7 +3329,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2708,13 +3395,13 @@
       <c r="D5" s="10">
         <v>2</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="26">
         <v>3</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="26">
         <v>4</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="26">
         <v>5</v>
       </c>
       <c r="H5" s="10">
@@ -2730,7 +3417,7 @@
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="24" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2773,16 +3460,16 @@
       <c r="D10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="29" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2799,16 +3486,16 @@
       <c r="D11" s="10">
         <v>2</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="27">
         <v>3</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="26">
         <v>4</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="26">
         <v>5</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="26">
         <v>6</v>
       </c>
     </row>
@@ -2821,7 +3508,7 @@
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="25" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2878,7 +3565,7 @@
       <c r="B18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -2935,7 +3622,7 @@
       <c r="C22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="10" t="s">
@@ -2958,10 +3645,10 @@
       <c r="B23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="10" t="s">
@@ -2986,7 +3673,7 @@
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="25" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3043,7 +3730,7 @@
       <c r="B30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="29" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="10" t="s">
@@ -3071,7 +3758,7 @@
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="25" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3134,7 +3821,7 @@
       <c r="B36" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="29" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="10" t="s">
@@ -3146,7 +3833,7 @@
       <c r="F36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="16" t="s">
+      <c r="G36" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H36" s="10" t="s">
@@ -3160,7 +3847,7 @@
       <c r="E38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="16" t="s">
+      <c r="G38" s="26" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3168,7 +3855,7 @@
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="25" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3225,7 +3912,7 @@
       <c r="B42" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="29" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="10" t="s">
@@ -3250,13 +3937,13 @@
       <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G45" s="16" t="s">
+      <c r="G45" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3319,7 +4006,7 @@
       <c r="B48" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="29" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -3331,7 +4018,7 @@
       <c r="F48" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="16" t="s">
+      <c r="G48" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H48" s="10" t="s">
@@ -3347,10 +4034,10 @@
       <c r="A51" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="30" t="s">
         <v>41</v>
       </c>
       <c r="G51" s="10" t="s">
@@ -3390,7 +4077,7 @@
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="30" t="s">
         <v>26</v>
       </c>
       <c r="C53" s="10" t="s">
@@ -3416,10 +4103,10 @@
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="29" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="10" t="s">
@@ -3451,10 +4138,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X167"/>
+  <dimension ref="A1:X229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2"/>
@@ -4707,19 +5394,15 @@
         <v>176</v>
       </c>
     </row>
-    <row r="137" ht="13.95" spans="5:11">
-      <c r="E137" s="12">
+    <row r="136" spans="3:3">
+      <c r="C136" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="138" ht="13.95" spans="5:11">
+      <c r="E138" s="14">
         <v>5</v>
       </c>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
-      <c r="H137" s="13"/>
-      <c r="I137" s="13"/>
-      <c r="J137" s="13"/>
-      <c r="K137" s="13"/>
-    </row>
-    <row r="138" ht="13.95" spans="5:11">
-      <c r="E138" s="13"/>
       <c r="F138" s="13"/>
       <c r="G138" s="13"/>
       <c r="H138" s="13"/>
@@ -4730,9 +5413,7 @@
     <row r="139" ht="13.95" spans="5:11">
       <c r="E139" s="13"/>
       <c r="F139" s="13"/>
-      <c r="G139" s="12">
-        <v>7</v>
-      </c>
+      <c r="G139" s="13"/>
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
       <c r="J139" s="13"/>
@@ -4741,7 +5422,9 @@
     <row r="140" ht="13.95" spans="5:11">
       <c r="E140" s="13"/>
       <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
+      <c r="G140" s="14">
+        <v>7</v>
+      </c>
       <c r="H140" s="13"/>
       <c r="I140" s="13"/>
       <c r="J140" s="13"/>
@@ -4752,9 +5435,7 @@
       <c r="F141" s="13"/>
       <c r="G141" s="13"/>
       <c r="H141" s="13"/>
-      <c r="I141" s="12">
-        <v>9</v>
-      </c>
+      <c r="I141" s="13"/>
       <c r="J141" s="13"/>
       <c r="K141" s="13"/>
     </row>
@@ -4763,7 +5444,9 @@
       <c r="F142" s="13"/>
       <c r="G142" s="13"/>
       <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
+      <c r="I142" s="14">
+        <v>9</v>
+      </c>
       <c r="J142" s="13"/>
       <c r="K142" s="13"/>
     </row>
@@ -4774,19 +5457,23 @@
       <c r="H143" s="13"/>
       <c r="I143" s="13"/>
       <c r="J143" s="13"/>
-      <c r="K143" s="12">
+      <c r="K143" s="13"/>
+    </row>
+    <row r="144" ht="13.95" spans="5:11">
+      <c r="E144" s="13"/>
+      <c r="F144" s="13"/>
+      <c r="G144" s="13"/>
+      <c r="H144" s="13"/>
+      <c r="I144" s="13"/>
+      <c r="J144" s="13"/>
+      <c r="K144" s="14">
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
-      <c r="A146" t="s">
-        <v>177</v>
-      </c>
-      <c r="B146" t="s">
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="147" spans="2:2">
       <c r="B147" t="s">
         <v>179</v>
       </c>
@@ -4801,15 +5488,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
-      <c r="A151" t="s">
+    <row r="150" spans="2:2">
+      <c r="B150" t="s">
         <v>182</v>
       </c>
-      <c r="B151" t="s">
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="152" spans="2:2">
       <c r="B152" t="s">
         <v>184</v>
       </c>
@@ -4824,93 +5511,580 @@
         <v>186</v>
       </c>
     </row>
-    <row r="155" spans="2:5">
+    <row r="155" spans="2:2">
       <c r="B155" t="s">
         <v>187</v>
       </c>
-      <c r="E155" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="156" spans="2:3">
+    </row>
+    <row r="156" spans="2:5">
       <c r="B156" t="s">
         <v>188</v>
       </c>
-      <c r="C156" t="s">
+      <c r="E156" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3">
+      <c r="B157" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="157" spans="2:5">
-      <c r="B157" t="s">
+      <c r="C157" t="s">
         <v>190</v>
-      </c>
-      <c r="C157"/>
-      <c r="E157" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="158" spans="2:5">
       <c r="B158" t="s">
         <v>191</v>
       </c>
+      <c r="C158"/>
       <c r="E158" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5">
+      <c r="B159" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="160" spans="2:3">
-      <c r="B160" t="s">
-        <v>121</v>
-      </c>
-      <c r="C160" t="s">
+      <c r="E159" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="161" spans="2:3">
       <c r="B161" t="s">
+        <v>121</v>
+      </c>
+      <c r="C161" t="s">
         <v>194</v>
       </c>
-      <c r="C161" t="s">
+    </row>
+    <row r="162" spans="2:3">
+      <c r="B162" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="162" spans="3:3">
       <c r="C162" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="163" spans="2:3">
-      <c r="B163" t="s">
+    <row r="163" spans="3:3">
+      <c r="C163" t="s">
         <v>197</v>
       </c>
-      <c r="C163" t="s">
+    </row>
+    <row r="164" spans="2:3">
+      <c r="B164" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="164" spans="3:3">
       <c r="C164" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="166" spans="2:10">
-      <c r="B166" t="s">
+    <row r="165" spans="3:3">
+      <c r="C165" t="s">
         <v>200</v>
       </c>
-      <c r="F166" t="s">
+    </row>
+    <row r="167" spans="2:10">
+      <c r="B167" t="s">
         <v>201</v>
       </c>
-      <c r="H166" t="s">
+      <c r="F167" t="s">
+        <v>202</v>
+      </c>
+      <c r="H167" t="s">
         <v>157</v>
       </c>
-      <c r="J166" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="167" spans="2:2">
-      <c r="B167" t="s">
+      <c r="J167" t="s">
         <v>203</v>
       </c>
     </row>
+    <row r="168" spans="2:2">
+      <c r="B168" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>205</v>
+      </c>
+      <c r="B170" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="174" spans="2:12">
+      <c r="B174" t="s">
+        <v>1</v>
+      </c>
+      <c r="D174" s="12">
+        <v>19</v>
+      </c>
+      <c r="E174" s="12">
+        <v>17</v>
+      </c>
+      <c r="F174" s="12">
+        <v>13</v>
+      </c>
+      <c r="G174" s="12">
+        <v>11</v>
+      </c>
+      <c r="H174" s="12">
+        <v>7</v>
+      </c>
+      <c r="I174" s="12">
+        <v>5</v>
+      </c>
+      <c r="J174" s="12">
+        <v>3</v>
+      </c>
+      <c r="K174" s="12">
+        <v>2</v>
+      </c>
+      <c r="L174" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="4:12">
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
+      <c r="F175" s="13"/>
+      <c r="G175" s="13"/>
+      <c r="H175" s="13"/>
+      <c r="I175" s="13"/>
+      <c r="J175" s="13"/>
+      <c r="K175" s="13"/>
+      <c r="L175" s="13"/>
+    </row>
+    <row r="176" spans="2:12">
+      <c r="B176" t="s">
+        <v>209</v>
+      </c>
+      <c r="D176" s="13">
+        <v>1</v>
+      </c>
+      <c r="E176" s="13">
+        <v>2</v>
+      </c>
+      <c r="F176" s="13">
+        <v>2</v>
+      </c>
+      <c r="G176" s="13">
+        <v>3</v>
+      </c>
+      <c r="H176" s="13">
+        <v>3</v>
+      </c>
+      <c r="I176" s="13">
+        <v>3</v>
+      </c>
+      <c r="J176" s="13">
+        <v>3</v>
+      </c>
+      <c r="K176" s="13">
+        <v>4</v>
+      </c>
+      <c r="L176" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="2:12">
+      <c r="B177" t="s">
+        <v>18</v>
+      </c>
+      <c r="D177" s="13">
+        <v>0</v>
+      </c>
+      <c r="E177" s="13">
+        <v>1</v>
+      </c>
+      <c r="F177" s="13">
+        <v>2</v>
+      </c>
+      <c r="G177" s="13">
+        <v>3</v>
+      </c>
+      <c r="H177" s="13">
+        <v>4</v>
+      </c>
+      <c r="I177" s="13">
+        <v>5</v>
+      </c>
+      <c r="J177" s="13">
+        <v>6</v>
+      </c>
+      <c r="K177" s="13">
+        <v>7</v>
+      </c>
+      <c r="L177" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" ht="13.95" spans="2:13">
+      <c r="B179" s="13"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
+      <c r="F179" s="13"/>
+      <c r="G179" s="13"/>
+      <c r="H179" s="14">
+        <v>19</v>
+      </c>
+      <c r="I179" s="13"/>
+      <c r="J179" s="13"/>
+      <c r="K179" s="13"/>
+      <c r="L179" s="13"/>
+      <c r="M179" s="13"/>
+    </row>
+    <row r="180" ht="13.95" spans="2:13">
+      <c r="B180" s="13"/>
+      <c r="C180" s="13"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
+      <c r="F180" s="13"/>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="13"/>
+      <c r="J180" s="13"/>
+      <c r="K180" s="13"/>
+      <c r="L180" s="13"/>
+      <c r="M180" s="13"/>
+    </row>
+    <row r="181" ht="13.95" spans="2:13">
+      <c r="B181" s="13"/>
+      <c r="C181" s="13"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="14">
+        <v>17</v>
+      </c>
+      <c r="F181" s="13"/>
+      <c r="G181" s="13"/>
+      <c r="H181" s="13"/>
+      <c r="I181" s="13"/>
+      <c r="J181" s="13"/>
+      <c r="K181" s="14">
+        <v>13</v>
+      </c>
+      <c r="L181" s="13"/>
+      <c r="M181" s="13"/>
+    </row>
+    <row r="182" ht="13.95" spans="2:13">
+      <c r="B182" s="13"/>
+      <c r="C182" s="13"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
+      <c r="F182" s="13"/>
+      <c r="G182" s="21"/>
+      <c r="H182" s="13"/>
+      <c r="I182" s="13"/>
+      <c r="J182" s="13"/>
+      <c r="K182" s="13"/>
+      <c r="L182" s="13"/>
+      <c r="M182" s="13"/>
+    </row>
+    <row r="183" ht="13.95" spans="2:13">
+      <c r="B183" s="13"/>
+      <c r="C183" s="14">
+        <v>11</v>
+      </c>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="13"/>
+      <c r="G183" s="14">
+        <v>7</v>
+      </c>
+      <c r="H183" s="13"/>
+      <c r="I183" s="14">
+        <v>5</v>
+      </c>
+      <c r="K183" s="13"/>
+      <c r="L183" s="13"/>
+      <c r="M183" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" ht="13.95" spans="2:13">
+      <c r="B184" s="13"/>
+      <c r="C184" s="13"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="13"/>
+      <c r="G184" s="13"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="13"/>
+      <c r="J184" s="13"/>
+      <c r="K184" s="13"/>
+      <c r="L184" s="13"/>
+      <c r="M184" s="13"/>
+    </row>
+    <row r="185" ht="13.95" spans="2:13">
+      <c r="B185" s="14">
+        <v>2</v>
+      </c>
+      <c r="C185" s="13"/>
+      <c r="D185" s="14">
+        <v>1</v>
+      </c>
+      <c r="E185" s="13"/>
+      <c r="F185" s="13"/>
+      <c r="G185" s="13"/>
+      <c r="H185" s="13"/>
+      <c r="I185" s="13"/>
+      <c r="J185" s="13"/>
+      <c r="K185" s="13"/>
+      <c r="L185" s="13"/>
+      <c r="M185" s="13"/>
+    </row>
+    <row r="188" spans="2:9">
+      <c r="B188" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C188" s="16"/>
+      <c r="F188" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G188" s="23"/>
+      <c r="I188" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="189" spans="2:9">
+      <c r="B189" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C189" s="18">
+        <v>11</v>
+      </c>
+      <c r="F189" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G189" s="18">
+        <v>7</v>
+      </c>
+      <c r="I189" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="190" ht="13.95" spans="2:7">
+      <c r="B190" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C190" s="18">
+        <v>2</v>
+      </c>
+      <c r="F190" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G190" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="2:3">
+      <c r="B191" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C191" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" ht="13.95" spans="2:3">
+      <c r="B192" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C192" s="20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>215</v>
+      </c>
+      <c r="B194" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2">
+      <c r="B195" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2">
+      <c r="B196" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4">
+      <c r="B197" t="s">
+        <v>219</v>
+      </c>
+      <c r="D197" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="198" spans="4:4">
+      <c r="D198" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="199" spans="4:4">
+      <c r="D199" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="200" spans="4:4">
+      <c r="D200" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="201" spans="4:4">
+      <c r="D201" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="203" spans="3:4">
+      <c r="C203" t="s">
+        <v>225</v>
+      </c>
+      <c r="D203" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="205" spans="4:5">
+      <c r="D205" t="s">
+        <v>227</v>
+      </c>
+      <c r="E205" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="206" spans="5:5">
+      <c r="E206" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="208" spans="4:5">
+      <c r="D208" t="s">
+        <v>230</v>
+      </c>
+      <c r="E208" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="209" spans="5:5">
+      <c r="E209" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="210" spans="5:5">
+      <c r="E210" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="212" spans="4:5">
+      <c r="D212" t="s">
+        <v>234</v>
+      </c>
+      <c r="E212" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="213" spans="5:5">
+      <c r="E213" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="214" spans="5:5">
+      <c r="E214" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="215" spans="5:5">
+      <c r="E215" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="217" spans="4:5">
+      <c r="D217" t="s">
+        <v>239</v>
+      </c>
+      <c r="E217" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="218" spans="5:5">
+      <c r="E218" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="219" spans="5:7">
+      <c r="E219" t="s">
+        <v>242</v>
+      </c>
+      <c r="G219" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="220" spans="5:5">
+      <c r="E220" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="222" spans="4:5">
+      <c r="D222" t="s">
+        <v>245</v>
+      </c>
+      <c r="E222" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="223" spans="5:5">
+      <c r="E223" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="224" spans="5:5">
+      <c r="E224" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="226" spans="4:4">
+      <c r="D226" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="227" spans="4:9">
+      <c r="D227" t="s">
+        <v>250</v>
+      </c>
+      <c r="G227" t="s">
+        <v>157</v>
+      </c>
+      <c r="I227" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="228" spans="4:4">
+      <c r="D228" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="229" spans="4:4">
+      <c r="D229" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="F188:G188"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added Running Time computation solution
</commit_message>
<xml_diff>
--- a/Data-structures.xlsx
+++ b/Data-structures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22152" windowHeight="10248" activeTab="1"/>
+    <workbookView windowWidth="22152" windowHeight="10248"/>
   </bookViews>
   <sheets>
     <sheet name="Data Structure" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="356">
   <si>
     <t>Array Data structure</t>
   </si>
@@ -147,6 +147,88 @@
   </si>
   <si>
     <t>Peek operation on the other hand just returns A from the head of the Queue, doesn't remove it.</t>
+  </si>
+  <si>
+    <t>How to Calculate Running Time of an algorithm?</t>
+  </si>
+  <si>
+    <t>Let's convert this flowchart to algorithm:</t>
+  </si>
+  <si>
+    <t>Step 1:</t>
+  </si>
+  <si>
+    <t>Take input n</t>
+  </si>
+  <si>
+    <t>Step 2:</t>
+  </si>
+  <si>
+    <t>Assign 0 to i</t>
+  </si>
+  <si>
+    <t>Step 3</t>
+  </si>
+  <si>
+    <t>Assign 1 to result</t>
+  </si>
+  <si>
+    <t>Step 4:</t>
+  </si>
+  <si>
+    <t>If i &lt; = n, continue, else jump to step 7</t>
+  </si>
+  <si>
+    <t>Step 5:</t>
+  </si>
+  <si>
+    <t>Multipy result with i. Assign the returned value to result.</t>
+  </si>
+  <si>
+    <t>Step 6:</t>
+  </si>
+  <si>
+    <t>Increment i and go to step 4.</t>
+  </si>
+  <si>
+    <t>Step 7:</t>
+  </si>
+  <si>
+    <t>Print result</t>
+  </si>
+  <si>
+    <t>Assumptions:</t>
+  </si>
+  <si>
+    <t>1. Cost of assignment, addition, comparison, increment is 1</t>
+  </si>
+  <si>
+    <t>2. Cost of taking input, printing output is 1.</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>No. of Times</t>
+  </si>
+  <si>
+    <t>Cost * Iterations</t>
+  </si>
+  <si>
+    <t>n+2</t>
+  </si>
+  <si>
+    <t>n+1</t>
+  </si>
+  <si>
+    <t>2n+2</t>
+  </si>
+  <si>
+    <t>Running Time T(n): 10 + 5n
+Complexity: O(n)</t>
   </si>
   <si>
     <t>Bubble Sort</t>
@@ -998,6 +1080,51 @@
   <si>
     <t>In order to look up for node degree or number of edges connected to particular node, the adjacency list will probably be fastest.</t>
   </si>
+  <si>
+    <t>Graph Traversal</t>
+  </si>
+  <si>
+    <t>DFS and BFS</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>Use Stacks</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>Use Queue</t>
+  </si>
+  <si>
+    <t>Eulerian Path</t>
+  </si>
+  <si>
+    <t>Each node should be visited only at once</t>
+  </si>
+  <si>
+    <t>To make this possible, each vertex should have only even number of edges. Starting and ending node can have odd number of edge.</t>
+  </si>
+  <si>
+    <t>Eulerian Cycle</t>
+  </si>
+  <si>
+    <t>Each node should should have even number of edges.</t>
+  </si>
+  <si>
+    <t>Hamiltonian Paths</t>
+  </si>
+  <si>
+    <t>A Hamiltonian path is another type of path that must go through every vertex once.</t>
+  </si>
+  <si>
+    <t>Hamiltonian Cycle</t>
+  </si>
+  <si>
+    <t>Similar to Eulerian Cycle</t>
+  </si>
 </sst>
 </file>
 
@@ -1005,8 +1132,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -1034,16 +1161,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1057,17 +1184,84 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1081,28 +1275,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1110,24 +1282,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1137,36 +1294,6 @@
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1251,13 +1378,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1269,7 +1426,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1287,19 +1468,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1311,7 +1486,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1323,114 +1552,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1810,6 +1937,114 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1829,56 +2064,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1907,147 +2092,197 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="35" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2057,7 +2292,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2151,79 +2386,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2430,6 +2722,48 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>213995</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>48260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="777240" y="10081260"/>
+          <a:ext cx="5723255" cy="3909695"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4170,7 +4504,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2689860" y="53568600"/>
+          <a:off x="2689860" y="53578125"/>
           <a:ext cx="678180" cy="184785"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4214,7 +4548,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3703320" y="53860065"/>
+          <a:off x="3703320" y="53869590"/>
           <a:ext cx="0" cy="346710"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4258,8 +4592,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2689860" y="54391560"/>
-          <a:ext cx="678180" cy="169545"/>
+          <a:off x="2689860" y="54401085"/>
+          <a:ext cx="678180" cy="177165"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4302,8 +4636,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2362200" y="53852445"/>
-          <a:ext cx="1005840" cy="708660"/>
+          <a:off x="2362200" y="53861970"/>
+          <a:ext cx="1005840" cy="716280"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4587,10 +4921,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2"/>
@@ -4600,6 +4934,7 @@
     <col min="3" max="3" width="8.8" style="10"/>
     <col min="4" max="4" width="10.3" style="10" customWidth="1"/>
     <col min="5" max="8" width="8.8" style="10"/>
+    <col min="13" max="13" width="9.8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -4611,7 +4946,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4677,13 +5012,13 @@
       <c r="D5" s="10">
         <v>2</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="48">
         <v>3</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="48">
         <v>4</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="48">
         <v>5</v>
       </c>
       <c r="H5" s="10">
@@ -4699,7 +5034,7 @@
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="46" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4742,16 +5077,16 @@
       <c r="D10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="54" t="s">
+      <c r="H10" s="51" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4768,16 +5103,16 @@
       <c r="D11" s="10">
         <v>2</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="49">
         <v>3</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="48">
         <v>4</v>
       </c>
-      <c r="G11" s="51">
+      <c r="G11" s="48">
         <v>5</v>
       </c>
-      <c r="H11" s="51">
+      <c r="H11" s="48">
         <v>6</v>
       </c>
     </row>
@@ -4790,7 +5125,7 @@
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="47" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4847,7 +5182,7 @@
       <c r="B18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="48" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -4904,7 +5239,7 @@
       <c r="C22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="49" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="10" t="s">
@@ -4927,10 +5262,10 @@
       <c r="B23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="48" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="10" t="s">
@@ -4955,7 +5290,7 @@
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="47" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5012,7 +5347,7 @@
       <c r="B30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="51" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="10" t="s">
@@ -5040,7 +5375,7 @@
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="47" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5103,7 +5438,7 @@
       <c r="B36" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C36" s="51" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="10" t="s">
@@ -5115,7 +5450,7 @@
       <c r="F36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="51" t="s">
+      <c r="G36" s="48" t="s">
         <v>10</v>
       </c>
       <c r="H36" s="10" t="s">
@@ -5129,7 +5464,7 @@
       <c r="E38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="51" t="s">
+      <c r="G38" s="48" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5137,7 +5472,7 @@
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="47" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5194,7 +5529,7 @@
       <c r="B42" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="51" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="10" t="s">
@@ -5219,13 +5554,13 @@
       <c r="A45" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="55" t="s">
+      <c r="D45" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G45" s="51" t="s">
+      <c r="G45" s="48" t="s">
         <v>38</v>
       </c>
     </row>
@@ -5288,7 +5623,7 @@
       <c r="B48" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="54" t="s">
+      <c r="C48" s="51" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -5300,7 +5635,7 @@
       <c r="F48" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="51" t="s">
+      <c r="G48" s="48" t="s">
         <v>10</v>
       </c>
       <c r="H48" s="10" t="s">
@@ -5316,10 +5651,10 @@
       <c r="A51" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="55" t="s">
+      <c r="D51" s="52" t="s">
         <v>41</v>
       </c>
       <c r="G51" s="10" t="s">
@@ -5359,7 +5694,7 @@
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="55" t="s">
+      <c r="B53" s="52" t="s">
         <v>26</v>
       </c>
       <c r="C53" s="10" t="s">
@@ -5385,10 +5720,10 @@
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="55" t="s">
+      <c r="B54" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="54" t="s">
+      <c r="C54" s="51" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="10" t="s">
@@ -5410,7 +5745,231 @@
         <v>43</v>
       </c>
     </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="10:10">
+      <c r="J59" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4">
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="10:11">
+      <c r="J61" t="s">
+        <v>46</v>
+      </c>
+      <c r="K61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="10:11">
+      <c r="J62" t="s">
+        <v>48</v>
+      </c>
+      <c r="K62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="10:11">
+      <c r="J63" t="s">
+        <v>50</v>
+      </c>
+      <c r="K63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="10:11">
+      <c r="J64" t="s">
+        <v>52</v>
+      </c>
+      <c r="K64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="10:11">
+      <c r="J65" t="s">
+        <v>54</v>
+      </c>
+      <c r="K65" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="10:11">
+      <c r="J66" t="s">
+        <v>56</v>
+      </c>
+      <c r="K66" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="10:11">
+      <c r="J67" t="s">
+        <v>58</v>
+      </c>
+      <c r="K67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="10:10">
+      <c r="J69" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="10:10">
+      <c r="J70" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="10:10">
+      <c r="J71" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" ht="40.35" spans="10:13">
+      <c r="J73" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="K73" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="L73" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="M73" s="68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="10:13">
+      <c r="J74" s="56">
+        <v>1</v>
+      </c>
+      <c r="K74" s="57">
+        <v>1</v>
+      </c>
+      <c r="L74" s="57">
+        <v>1</v>
+      </c>
+      <c r="M74" s="69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="10:13">
+      <c r="J75" s="58">
+        <v>2</v>
+      </c>
+      <c r="K75" s="59">
+        <v>1</v>
+      </c>
+      <c r="L75" s="59">
+        <v>1</v>
+      </c>
+      <c r="M75" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="10:13">
+      <c r="J76" s="58">
+        <v>3</v>
+      </c>
+      <c r="K76" s="59">
+        <v>1</v>
+      </c>
+      <c r="L76" s="59">
+        <v>1</v>
+      </c>
+      <c r="M76" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="10:13">
+      <c r="J77" s="58">
+        <v>4</v>
+      </c>
+      <c r="K77" s="59">
+        <v>1</v>
+      </c>
+      <c r="L77" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="M77" s="70" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="10:13">
+      <c r="J78" s="58">
+        <v>5</v>
+      </c>
+      <c r="K78" s="59">
+        <v>2</v>
+      </c>
+      <c r="L78" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="M78" s="70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="10:13">
+      <c r="J79" s="58">
+        <v>6</v>
+      </c>
+      <c r="K79" s="59">
+        <v>2</v>
+      </c>
+      <c r="L79" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="M79" s="70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" ht="13.95" spans="10:13">
+      <c r="J80" s="60">
+        <v>7</v>
+      </c>
+      <c r="K80" s="61">
+        <v>1</v>
+      </c>
+      <c r="L80" s="61">
+        <v>1</v>
+      </c>
+      <c r="M80" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" ht="13.95" spans="10:12">
+      <c r="J81" s="62"/>
+      <c r="K81" s="62"/>
+      <c r="L81" s="62"/>
+    </row>
+    <row r="82" spans="10:13">
+      <c r="J82" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="K82" s="64"/>
+      <c r="L82" s="64"/>
+      <c r="M82" s="72"/>
+    </row>
+    <row r="83" spans="10:13">
+      <c r="J83" s="65"/>
+      <c r="K83" s="62"/>
+      <c r="L83" s="62"/>
+      <c r="M83" s="73"/>
+    </row>
+    <row r="84" spans="10:13">
+      <c r="J84" s="66"/>
+      <c r="K84" s="67"/>
+      <c r="L84" s="67"/>
+      <c r="M84" s="74"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J82:M84"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
@@ -5420,10 +5979,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:X325"/>
+  <dimension ref="A1:X338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="B327" sqref="B327"/>
+    <sheetView topLeftCell="A308" workbookViewId="0">
+      <selection activeCell="B339" sqref="B339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2"/>
@@ -5436,12 +5995,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -5461,15 +6020,15 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="M5" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -5480,7 +6039,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -5489,18 +6048,18 @@
         <v>7</v>
       </c>
       <c r="M8" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="N8">
         <v>5</v>
       </c>
       <c r="O8" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -5509,18 +6068,18 @@
         <v>7</v>
       </c>
       <c r="M9" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -5529,29 +6088,29 @@
         <v>8</v>
       </c>
       <c r="M10" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="N10">
         <v>4</v>
       </c>
       <c r="O10" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="13:15">
       <c r="M11" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="N11" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="O11" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>
@@ -5569,28 +6128,28 @@
         <v>8</v>
       </c>
       <c r="M12" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="O12" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="13:15">
       <c r="M13" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="O13" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -5601,7 +6160,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -5612,7 +6171,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -5623,7 +6182,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E19">
         <v>7</v>
@@ -5634,7 +6193,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -5654,12 +6213,12 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -5670,7 +6229,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -5681,7 +6240,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -5692,7 +6251,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E28">
         <v>7</v>
@@ -5703,7 +6262,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
@@ -5723,12 +6282,12 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5739,7 +6298,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -5750,7 +6309,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -5761,7 +6320,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="E37">
         <v>7</v>
@@ -5772,7 +6331,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -5792,20 +6351,20 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B46">
         <v>9</v>
@@ -5838,75 +6397,75 @@
         <v>4</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="N46" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="13:14">
       <c r="M47" s="1" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="N47" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="F48" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="H48" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="J48" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="N48" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="F49" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="N49" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B50" s="5">
         <v>1</v>
@@ -5924,54 +6483,54 @@
         <v>1</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="N50" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="13:15">
       <c r="M51" s="1" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="N51" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="O51" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="F52" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="J52" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="J53" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -5985,16 +6544,16 @@
     </row>
     <row r="56" spans="1:24">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="J56" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -6032,16 +6591,16 @@
     </row>
     <row r="57" spans="1:24">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="J57" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="N57">
         <v>0</v>
@@ -6079,7 +6638,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B58">
         <v>7</v>
@@ -6090,23 +6649,23 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="B62">
         <v>9</v>
@@ -6114,20 +6673,20 @@
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -6135,7 +6694,7 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="B69" s="4">
         <v>8</v>
@@ -6161,7 +6720,7 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="B70" s="6">
         <v>10</v>
@@ -6187,7 +6746,7 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="B71" s="7">
         <v>0</v>
@@ -6213,7 +6772,7 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -6239,7 +6798,7 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -6265,136 +6824,136 @@
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" t="s">
+        <v>141</v>
+      </c>
+      <c r="C82" t="s">
+        <v>142</v>
+      </c>
+      <c r="D82" t="s">
+        <v>143</v>
+      </c>
+      <c r="F82" t="s">
+        <v>144</v>
+      </c>
+      <c r="H82" t="s">
         <v>113</v>
       </c>
-      <c r="B82" t="s">
-        <v>114</v>
-      </c>
-      <c r="C82" t="s">
-        <v>115</v>
-      </c>
-      <c r="D82" t="s">
-        <v>116</v>
-      </c>
-      <c r="F82" t="s">
-        <v>117</v>
-      </c>
-      <c r="H82" t="s">
-        <v>86</v>
-      </c>
       <c r="I82" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="2:9">
       <c r="B83" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="C83" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="D83" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="F83" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="H83" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="I83" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="B84" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C84" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="D84" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="B85" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="C85" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="D85" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="B87" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="D87" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="B88" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" spans="4:4">
       <c r="D89" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
     </row>
     <row r="90" spans="4:4">
       <c r="D90" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="4:4">
       <c r="D91" s="1" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="4:4">
       <c r="D92" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" spans="4:4">
       <c r="D93" s="1" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" ht="13.95" spans="4:9">
@@ -6431,7 +6990,7 @@
       <c r="E98" s="10"/>
       <c r="G98" s="10"/>
       <c r="H98" s="11" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="I98" s="10"/>
     </row>
@@ -6452,133 +7011,133 @@
         <v>14</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="11" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="3:4">
       <c r="C103" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="D103" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
     </row>
     <row r="104" spans="3:4">
       <c r="C104" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="D104" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="3:4">
       <c r="C105" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="D105" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="B107" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="2:11">
       <c r="B108" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="D108" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="K108" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="109" spans="2:15">
       <c r="B109" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="D109" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="O109" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="2:4">
       <c r="B110" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="D110" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
     </row>
     <row r="111" spans="4:10">
       <c r="D111" t="s">
-        <v>156</v>
+        <v>183</v>
       </c>
       <c r="J111" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
     </row>
     <row r="113" spans="2:4">
       <c r="B113" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="D113" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
     </row>
     <row r="114" spans="4:4">
       <c r="D114" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="B116" t="s">
-        <v>162</v>
+        <v>189</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
       <c r="C118" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
     </row>
     <row r="121" spans="3:7">
       <c r="C121" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="G121" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" t="s">
-        <v>168</v>
+        <v>195</v>
       </c>
     </row>
     <row r="123" ht="13.95"/>
@@ -6638,47 +7197,47 @@
     </row>
     <row r="131" spans="1:11">
       <c r="A131" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="C131" t="s">
-        <v>170</v>
+        <v>197</v>
       </c>
       <c r="G131" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="H131" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="J131" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="K131" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
     </row>
     <row r="137" ht="13.95"/>
@@ -6755,151 +7314,151 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="B147" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
     </row>
     <row r="148" spans="2:2">
       <c r="B148" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
     </row>
     <row r="149" spans="2:2">
       <c r="B149" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
     </row>
     <row r="150" spans="2:2">
       <c r="B150" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="B152" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
     </row>
     <row r="153" spans="2:2">
       <c r="B153" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
     </row>
     <row r="154" spans="2:2">
       <c r="B154" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
     </row>
     <row r="155" spans="2:2">
       <c r="B155" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
     </row>
     <row r="156" spans="2:5">
       <c r="B156" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="E156" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="157" spans="2:3">
       <c r="B157" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="C157" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="158" spans="2:5">
       <c r="B158" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="E158" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="159" spans="2:5">
       <c r="B159" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="E159" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
     </row>
     <row r="161" spans="2:3">
       <c r="B161" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="C161" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
     </row>
     <row r="162" spans="2:3">
       <c r="B162" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="C162" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
     </row>
     <row r="163" spans="3:3">
       <c r="C163" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
     </row>
     <row r="164" spans="2:3">
       <c r="B164" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="C164" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
     </row>
     <row r="165" spans="3:3">
       <c r="C165" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
     </row>
     <row r="167" spans="2:10">
       <c r="B167" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="F167" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
       <c r="H167" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="J167" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
     </row>
     <row r="168" spans="2:2">
       <c r="B168" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="B170" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
     </row>
     <row r="171" spans="2:2">
       <c r="B171" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
     </row>
     <row r="172" spans="2:2">
       <c r="B172" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
     </row>
     <row r="174" spans="2:12">
@@ -6947,7 +7506,7 @@
     </row>
     <row r="176" spans="2:12">
       <c r="B176" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="D176" s="10">
         <v>1</v>
@@ -7128,7 +7687,7 @@
     <row r="187" ht="13.95"/>
     <row r="188" spans="2:9">
       <c r="B188" s="13" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="C188" s="14"/>
       <c r="F188" s="20" t="s">
@@ -7136,7 +7695,7 @@
       </c>
       <c r="G188" s="21"/>
       <c r="I188" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
     </row>
     <row r="189" spans="2:9">
@@ -7153,12 +7712,12 @@
         <v>7</v>
       </c>
       <c r="I189" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
     </row>
     <row r="190" ht="13.95" spans="2:7">
       <c r="B190" s="15" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="C190" s="16">
         <v>2</v>
@@ -7172,7 +7731,7 @@
     </row>
     <row r="191" spans="2:3">
       <c r="B191" s="15" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="C191" s="16">
         <v>1</v>
@@ -7180,7 +7739,7 @@
     </row>
     <row r="192" ht="13.95" spans="2:3">
       <c r="B192" s="17" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C192" s="18">
         <v>17</v>
@@ -7188,180 +7747,180 @@
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="B194" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
     </row>
     <row r="195" spans="2:2">
       <c r="B195" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
     </row>
     <row r="196" spans="2:2">
       <c r="B196" t="s">
-        <v>218</v>
+        <v>245</v>
       </c>
     </row>
     <row r="197" spans="2:4">
       <c r="B197" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
       <c r="D197" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
     </row>
     <row r="198" spans="4:4">
       <c r="D198" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
     </row>
     <row r="199" spans="4:4">
       <c r="D199" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
     </row>
     <row r="200" spans="4:4">
       <c r="D200" t="s">
-        <v>223</v>
+        <v>250</v>
       </c>
     </row>
     <row r="201" spans="4:4">
       <c r="D201" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
     </row>
     <row r="203" spans="3:4">
       <c r="C203" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="D203" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
     </row>
     <row r="205" spans="4:5">
       <c r="D205" t="s">
-        <v>227</v>
+        <v>254</v>
       </c>
       <c r="E205" t="s">
-        <v>228</v>
+        <v>255</v>
       </c>
     </row>
     <row r="206" spans="5:5">
       <c r="E206" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
     </row>
     <row r="208" spans="4:5">
       <c r="D208" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="E208" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
     </row>
     <row r="209" spans="5:5">
       <c r="E209" t="s">
-        <v>232</v>
+        <v>259</v>
       </c>
     </row>
     <row r="210" spans="5:5">
       <c r="E210" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
     </row>
     <row r="212" spans="4:5">
       <c r="D212" t="s">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="E212" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
     </row>
     <row r="213" spans="5:5">
       <c r="E213" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
     </row>
     <row r="214" spans="5:5">
       <c r="E214" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
     </row>
     <row r="215" spans="5:5">
       <c r="E215" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
     </row>
     <row r="217" spans="4:5">
       <c r="D217" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="E217" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
     </row>
     <row r="218" spans="5:5">
       <c r="E218" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
     </row>
     <row r="219" spans="5:7">
       <c r="E219" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="G219" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
     </row>
     <row r="220" spans="5:5">
       <c r="E220" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
     </row>
     <row r="222" spans="4:5">
       <c r="D222" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="E222" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
     </row>
     <row r="223" spans="5:5">
       <c r="E223" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
     </row>
     <row r="224" spans="5:5">
       <c r="E224" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
     </row>
     <row r="226" spans="4:4">
       <c r="D226" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
     </row>
     <row r="227" spans="4:9">
       <c r="D227" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="G227" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="I227" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="228" spans="4:4">
       <c r="D228" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
     </row>
     <row r="229" spans="4:4">
       <c r="D229" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
     </row>
     <row r="231" ht="13.95"/>
@@ -7472,505 +8031,568 @@
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="B242" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
     </row>
     <row r="243" spans="2:2">
       <c r="B243" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
     </row>
     <row r="244" spans="2:2">
       <c r="B244" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
     </row>
     <row r="245" spans="2:2">
       <c r="B245" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
     </row>
     <row r="246" spans="2:2">
       <c r="B246" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
     </row>
     <row r="247" spans="2:2">
       <c r="B247" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
     </row>
     <row r="248" spans="2:2">
       <c r="B248" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
     </row>
     <row r="249" spans="2:2">
       <c r="B249" t="s">
-        <v>262</v>
+        <v>289</v>
       </c>
     </row>
     <row r="250" spans="2:2">
       <c r="B250" t="s">
-        <v>263</v>
+        <v>290</v>
       </c>
     </row>
     <row r="251" spans="2:2">
       <c r="B251" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="B253" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
     </row>
     <row r="254" spans="2:2">
       <c r="B254" t="s">
-        <v>267</v>
+        <v>294</v>
       </c>
     </row>
     <row r="255" spans="2:2">
       <c r="B255" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
     </row>
     <row r="256" spans="2:2">
       <c r="B256" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>270</v>
+        <v>297</v>
       </c>
       <c r="C258" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
       <c r="B260" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
     </row>
     <row r="261" spans="2:2">
       <c r="B261" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" t="s">
-        <v>275</v>
+        <v>302</v>
       </c>
       <c r="B263" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="B265" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
     </row>
     <row r="266" spans="2:2">
       <c r="B266" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
       <c r="B268" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="269" spans="2:2">
       <c r="B269" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" t="s">
-        <v>283</v>
+        <v>310</v>
       </c>
       <c r="B271" t="s">
-        <v>284</v>
+        <v>311</v>
       </c>
     </row>
     <row r="273" ht="13.95" spans="1:3">
       <c r="A273" t="s">
-        <v>285</v>
+        <v>312</v>
       </c>
       <c r="C273" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
     </row>
     <row r="274" spans="3:5">
       <c r="C274" s="28" t="s">
-        <v>287</v>
+        <v>314</v>
       </c>
       <c r="E274" s="28" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
     </row>
     <row r="275" spans="3:5">
       <c r="C275" s="29" t="s">
-        <v>289</v>
+        <v>316</v>
       </c>
       <c r="E275" s="29" t="s">
-        <v>290</v>
+        <v>317</v>
       </c>
     </row>
     <row r="276" spans="3:5">
       <c r="C276" s="29" t="s">
-        <v>291</v>
+        <v>318</v>
       </c>
       <c r="E276" s="29" t="s">
-        <v>291</v>
+        <v>318</v>
       </c>
     </row>
     <row r="277" ht="13.95" spans="3:5">
       <c r="C277" s="30" t="s">
-        <v>292</v>
+        <v>319</v>
       </c>
       <c r="E277" s="30" t="s">
-        <v>293</v>
+        <v>320</v>
       </c>
     </row>
     <row r="279" spans="3:3">
       <c r="C279" t="s">
-        <v>294</v>
+        <v>321</v>
       </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="B281" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
     </row>
     <row r="282" spans="2:2">
       <c r="B282" t="s">
-        <v>297</v>
+        <v>324</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
     </row>
     <row r="284" spans="2:2">
       <c r="B284" t="s">
-        <v>299</v>
+        <v>326</v>
       </c>
     </row>
     <row r="286" ht="13.95"/>
     <row r="287" ht="13.95" spans="2:7">
-      <c r="B287" s="31">
+      <c r="B287" s="11">
         <v>0</v>
       </c>
-      <c r="C287" s="32"/>
-      <c r="D287" s="32"/>
+      <c r="C287" s="10"/>
+      <c r="D287" s="10"/>
       <c r="G287" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
     </row>
     <row r="288" ht="13.95" spans="2:4">
-      <c r="B288" s="32"/>
-      <c r="C288" s="32"/>
-      <c r="D288" s="32"/>
+      <c r="B288" s="10"/>
+      <c r="C288" s="10"/>
+      <c r="D288" s="10"/>
     </row>
     <row r="289" ht="13.95" spans="2:12">
-      <c r="B289" s="32"/>
-      <c r="C289" s="32"/>
-      <c r="D289" s="31">
+      <c r="B289" s="10"/>
+      <c r="C289" s="10"/>
+      <c r="D289" s="11">
         <v>1</v>
       </c>
       <c r="G289" t="s">
         <v>1</v>
       </c>
-      <c r="I289" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="J289" s="32" t="s">
-        <v>302</v>
-      </c>
-      <c r="K289" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="L289" s="32" t="s">
-        <v>304</v>
+      <c r="I289" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="J289" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="K289" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="L289" s="10" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="290" spans="2:12">
-      <c r="B290" s="32"/>
-      <c r="C290" s="32"/>
-      <c r="D290" s="32"/>
+      <c r="B290" s="10"/>
+      <c r="C290" s="10"/>
+      <c r="D290" s="10"/>
       <c r="G290" t="s">
         <v>18</v>
       </c>
-      <c r="I290" s="32">
+      <c r="I290" s="10">
         <v>0</v>
       </c>
-      <c r="J290" s="32">
+      <c r="J290" s="10">
         <v>1</v>
       </c>
-      <c r="K290" s="32">
+      <c r="K290" s="10">
         <v>2</v>
       </c>
-      <c r="L290" s="32">
+      <c r="L290" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="291" spans="2:4">
-      <c r="B291" s="32"/>
-      <c r="C291" s="32"/>
-      <c r="D291" s="32"/>
+      <c r="B291" s="10"/>
+      <c r="C291" s="10"/>
+      <c r="D291" s="10"/>
     </row>
     <row r="292" ht="13.95" spans="2:4">
-      <c r="B292" s="32"/>
-      <c r="C292" s="32"/>
-      <c r="D292" s="32"/>
+      <c r="B292" s="10"/>
+      <c r="C292" s="10"/>
+      <c r="D292" s="10"/>
     </row>
     <row r="293" ht="13.95" spans="2:4">
-      <c r="B293" s="32"/>
-      <c r="C293" s="32"/>
-      <c r="D293" s="31">
+      <c r="B293" s="10"/>
+      <c r="C293" s="10"/>
+      <c r="D293" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="294" ht="13.95" spans="2:4">
-      <c r="B294" s="32"/>
-      <c r="C294" s="32"/>
-      <c r="D294" s="32"/>
+      <c r="B294" s="10"/>
+      <c r="C294" s="10"/>
+      <c r="D294" s="10"/>
     </row>
     <row r="295" ht="13.95" spans="2:4">
-      <c r="B295" s="31">
+      <c r="B295" s="11">
         <v>2</v>
       </c>
-      <c r="C295" s="32"/>
-      <c r="D295" s="32"/>
+      <c r="C295" s="10"/>
+      <c r="D295" s="10"/>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
       <c r="B298" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
     </row>
     <row r="299" spans="2:2">
       <c r="B299" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
     </row>
     <row r="301" ht="13.95" spans="4:7">
-      <c r="D301" s="32"/>
-      <c r="E301" s="32"/>
+      <c r="D301" s="10"/>
+      <c r="E301" s="10"/>
       <c r="G301" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
     </row>
     <row r="302" ht="13.95" spans="3:4">
-      <c r="C302" s="31">
+      <c r="C302" s="11">
         <v>0</v>
       </c>
-      <c r="D302" s="32"/>
+      <c r="D302" s="10"/>
     </row>
     <row r="303" ht="13.95" spans="3:12">
-      <c r="C303" s="32"/>
-      <c r="D303" s="32"/>
-      <c r="E303" s="31">
+      <c r="C303" s="10"/>
+      <c r="D303" s="10"/>
+      <c r="E303" s="11">
         <v>1</v>
       </c>
       <c r="G303" t="s">
         <v>1</v>
       </c>
-      <c r="I303" s="32" t="s">
-        <v>309</v>
-      </c>
-      <c r="J303" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="K303" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="L303" s="32" t="s">
-        <v>302</v>
+      <c r="I303" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="J303" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="K303" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="L303" s="10" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="304" spans="3:12">
-      <c r="C304" s="32"/>
-      <c r="D304" s="32"/>
-      <c r="E304" s="32"/>
+      <c r="C304" s="10"/>
+      <c r="D304" s="10"/>
+      <c r="E304" s="10"/>
       <c r="G304" t="s">
         <v>18</v>
       </c>
-      <c r="I304" s="32">
+      <c r="I304" s="10">
         <v>0</v>
       </c>
-      <c r="J304" s="32">
+      <c r="J304" s="10">
         <v>1</v>
       </c>
-      <c r="K304" s="32">
+      <c r="K304" s="10">
         <v>2</v>
       </c>
-      <c r="L304" s="32">
+      <c r="L304" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="305" ht="13.95" spans="3:5">
-      <c r="C305" s="32"/>
-      <c r="D305" s="32"/>
-      <c r="E305" s="32"/>
+      <c r="C305" s="10"/>
+      <c r="D305" s="10"/>
+      <c r="E305" s="10"/>
     </row>
     <row r="306" ht="13.95" spans="4:5">
-      <c r="D306" s="32"/>
-      <c r="E306" s="31">
+      <c r="D306" s="10"/>
+      <c r="E306" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="307" ht="13.95"/>
     <row r="308" ht="13.95" spans="3:3">
-      <c r="C308" s="31">
+      <c r="C308" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="A311" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="B311" t="s">
-        <v>312</v>
-      </c>
-    </row>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="314" ht="13.95"/>
     <row r="315" ht="13.95" spans="7:11">
-      <c r="G315" s="33"/>
-      <c r="H315" s="34">
+      <c r="G315" s="31"/>
+      <c r="H315" s="32">
         <v>0</v>
       </c>
-      <c r="I315" s="41">
+      <c r="I315" s="39">
         <v>1</v>
       </c>
-      <c r="J315" s="41">
+      <c r="J315" s="39">
         <v>2</v>
       </c>
-      <c r="K315" s="42">
+      <c r="K315" s="40">
         <v>3</v>
       </c>
     </row>
     <row r="316" ht="13.95" spans="7:11">
-      <c r="G316" s="35">
+      <c r="G316" s="33">
         <v>0</v>
       </c>
-      <c r="H316" s="36">
+      <c r="H316" s="34">
         <v>0</v>
       </c>
-      <c r="I316" s="43">
+      <c r="I316" s="41">
         <v>1</v>
       </c>
-      <c r="J316" s="43">
+      <c r="J316" s="41">
         <v>0</v>
       </c>
-      <c r="K316" s="44">
+      <c r="K316" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="317" ht="13.95" spans="3:11">
-      <c r="C317" s="31">
+      <c r="C317" s="11">
         <v>0</v>
       </c>
-      <c r="D317" s="32"/>
-      <c r="G317" s="37">
+      <c r="D317" s="10"/>
+      <c r="G317" s="35">
         <v>1</v>
       </c>
-      <c r="H317" s="38">
+      <c r="H317" s="36">
         <v>1</v>
       </c>
-      <c r="I317" s="45">
+      <c r="I317" s="12">
         <v>0</v>
       </c>
-      <c r="J317" s="45">
+      <c r="J317" s="12">
         <v>1</v>
       </c>
-      <c r="K317" s="46">
+      <c r="K317" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="318" ht="13.95" spans="3:11">
-      <c r="C318" s="32"/>
-      <c r="D318" s="32"/>
-      <c r="E318" s="31">
+      <c r="C318" s="10"/>
+      <c r="D318" s="10"/>
+      <c r="E318" s="11">
         <v>1</v>
       </c>
-      <c r="G318" s="37">
+      <c r="G318" s="35">
         <v>2</v>
       </c>
-      <c r="H318" s="38">
+      <c r="H318" s="36">
         <v>0</v>
       </c>
-      <c r="I318" s="45">
+      <c r="I318" s="12">
         <v>1</v>
       </c>
-      <c r="J318" s="45">
+      <c r="J318" s="12">
         <v>0</v>
       </c>
-      <c r="K318" s="46">
+      <c r="K318" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="319" ht="13.95" spans="3:11">
-      <c r="C319" s="32"/>
-      <c r="D319" s="32"/>
-      <c r="E319" s="32"/>
-      <c r="G319" s="39">
+      <c r="C319" s="10"/>
+      <c r="D319" s="10"/>
+      <c r="E319" s="10"/>
+      <c r="G319" s="37">
         <v>3</v>
       </c>
-      <c r="H319" s="40">
+      <c r="H319" s="38">
         <v>0</v>
       </c>
-      <c r="I319" s="47">
+      <c r="I319" s="44">
         <v>1</v>
       </c>
-      <c r="J319" s="47">
+      <c r="J319" s="44">
         <v>1</v>
       </c>
-      <c r="K319" s="48">
+      <c r="K319" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="320" ht="13.95" spans="3:5">
-      <c r="C320" s="32"/>
-      <c r="D320" s="32"/>
-      <c r="E320" s="32"/>
+      <c r="C320" s="10"/>
+      <c r="D320" s="10"/>
+      <c r="E320" s="10"/>
     </row>
     <row r="321" ht="13.95" spans="4:5">
-      <c r="D321" s="32"/>
-      <c r="E321" s="31">
+      <c r="D321" s="10"/>
+      <c r="E321" s="11">
         <v>2</v>
       </c>
     </row>
+    <row r="322" ht="13.95"/>
     <row r="323" ht="13.95" spans="3:3">
-      <c r="C323" s="31">
+      <c r="C323" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="325" spans="2:2">
       <c r="B325" t="s">
-        <v>313</v>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
+      <c r="A327" t="s">
+        <v>341</v>
+      </c>
+      <c r="B327" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="328" spans="2:3">
+      <c r="B328" t="s">
+        <v>343</v>
+      </c>
+      <c r="C328" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="329" spans="2:3">
+      <c r="B329" t="s">
+        <v>345</v>
+      </c>
+      <c r="C329" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
+      <c r="A331" t="s">
+        <v>347</v>
+      </c>
+      <c r="B331" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="332" spans="2:2">
+      <c r="B332" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" t="s">
+        <v>350</v>
+      </c>
+      <c r="B334" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" t="s">
+        <v>352</v>
+      </c>
+      <c r="B336" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
+      <c r="A338" t="s">
+        <v>354</v>
+      </c>
+      <c r="B338" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>